<commit_message>
fixed small bug in data file header, cleaned notebook
</commit_message>
<xml_diff>
--- a/Clean/June2016/report3_po_witness.xlsx
+++ b/Clean/June2016/report3_po_witness.xlsx
@@ -19,22 +19,22 @@
     <t>Complaint_Number</t>
   </si>
   <si>
-    <t>PO_Witness_PO_Witness_Name</t>
-  </si>
-  <si>
-    <t>PO_Witness_PO_Witness_Gender</t>
-  </si>
-  <si>
-    <t>PO_Witness_PO_Witness_Race</t>
-  </si>
-  <si>
-    <t>PO_Witness_PO_Witness_Star</t>
-  </si>
-  <si>
-    <t>PO_Witness_PO_Witness_Birth_Year</t>
-  </si>
-  <si>
-    <t>PO_Witness_PO_Witness_Date_Appointed</t>
+    <t>PO_Witness_Name</t>
+  </si>
+  <si>
+    <t>PO_Witness_Gender</t>
+  </si>
+  <si>
+    <t>PO_Witness_Race</t>
+  </si>
+  <si>
+    <t>PO_Witness_Star</t>
+  </si>
+  <si>
+    <t>PO_Witness_Birth_Year</t>
+  </si>
+  <si>
+    <t>PO_Witness_Date_Appointed</t>
   </si>
   <si>
     <t>1053502</t>

</xml_diff>